<commit_message>
updated euro tie break code
</commit_message>
<xml_diff>
--- a/data/tb_wc.xlsx
+++ b/data/tb_wc.xlsx
@@ -1874,13 +1874,13 @@
         <v>1</v>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
       </c>
       <c r="H45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
@@ -1967,7 +1967,7 @@
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
         <v>1</v>
@@ -1976,7 +1976,7 @@
         <v>1</v>
       </c>
       <c r="H48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -8876,7 +8876,7 @@
         </is>
       </c>
       <c r="D264" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E264" t="n">
         <v>0</v>
@@ -8888,7 +8888,7 @@
         <v>0</v>
       </c>
       <c r="H264" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="265">
@@ -8914,13 +8914,13 @@
         <v>2</v>
       </c>
       <c r="F265" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G265" t="n">
         <v>0</v>
       </c>
       <c r="H265" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="266">
@@ -8943,7 +8943,7 @@
         <v>0</v>
       </c>
       <c r="E266" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F266" t="n">
         <v>2</v>
@@ -8952,7 +8952,7 @@
         <v>0</v>
       </c>
       <c r="H266" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="267">
@@ -8981,10 +8981,10 @@
         <v>0</v>
       </c>
       <c r="G267" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H267" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="268">

</xml_diff>